<commit_message>
12/04 carga de archivos
</commit_message>
<xml_diff>
--- a/Adm_recursos/Analisis_Cierre_ADM_Obligaciones.xlsx
+++ b/Adm_recursos/Analisis_Cierre_ADM_Obligaciones.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="55">
   <si>
     <t>05718d8 10/04 add logic progress bar FrmObligaciones v4.9.832  0.5h</t>
   </si>
@@ -154,16 +154,44 @@
   </si>
   <si>
     <t xml:space="preserve">Desvio </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Cambio en la cuenta corriente  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Tarifas precio + peaje =&gt; Total </t>
+  </si>
+  <si>
+    <t>Obligacion habilitar el por licenciatario</t>
+  </si>
+  <si>
+    <t>Permitir el cobrar el cobro de un ticket de un licenciatario por otro</t>
+  </si>
+  <si>
+    <t>Facturado &lt;&gt; Pagado</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Utilitario  </t>
+  </si>
+  <si>
+    <t>Hora disposicion</t>
+  </si>
+  <si>
+    <t>Peaje</t>
+  </si>
+  <si>
+    <t>modificaciones a factura, que el peaje sea una linea</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <numFmts count="1">
+  <numFmts count="2">
+    <numFmt numFmtId="44" formatCode="_-&quot;$&quot;\ * #,##0.00_-;\-&quot;$&quot;\ * #,##0.00_-;_-&quot;$&quot;\ * &quot;-&quot;??_-;_-@_-"/>
     <numFmt numFmtId="164" formatCode="0.0"/>
   </numFmts>
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -191,6 +219,13 @@
       <b/>
       <sz val="11"/>
       <color theme="3" tint="0.39997558519241921"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -234,10 +269,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="44" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
@@ -248,11 +284,14 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="44" fontId="1" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="44" fontId="3" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="44" fontId="2" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Moneda" xfId="1" builtinId="4"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -552,16 +591,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:C70"/>
+  <dimension ref="B2:C83"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A49" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="B70" sqref="B70"/>
+    <sheetView tabSelected="1" topLeftCell="A70" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="B83" sqref="B83"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="3.21875" customWidth="1"/>
-    <col min="2" max="2" width="89" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="88.5546875" customWidth="1"/>
     <col min="3" max="3" width="20.5546875" style="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -1088,7 +1127,7 @@
       <c r="B67" s="5" t="s">
         <v>42</v>
       </c>
-      <c r="C67" s="6">
+      <c r="C67" s="11">
         <v>590</v>
       </c>
     </row>
@@ -1096,7 +1135,7 @@
       <c r="B68" s="5" t="s">
         <v>43</v>
       </c>
-      <c r="C68" s="6">
+      <c r="C68" s="11">
         <f>C66*C67</f>
         <v>22420</v>
       </c>
@@ -1105,17 +1144,65 @@
       <c r="B69" s="5" t="s">
         <v>44</v>
       </c>
-      <c r="C69" s="10">
+      <c r="C69" s="12">
         <v>14700</v>
       </c>
     </row>
     <row r="70" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B70" s="11" t="s">
+      <c r="B70" s="10" t="s">
         <v>45</v>
       </c>
-      <c r="C70" s="12">
+      <c r="C70" s="13">
         <f>C68-C69</f>
         <v>7720</v>
+      </c>
+    </row>
+    <row r="73" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B73" s="14" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="74" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B74" s="14" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="75" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B75" s="14" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="76" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B76" s="14"/>
+    </row>
+    <row r="77" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B77" s="14" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="78" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B78" s="14" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="79" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B79" s="14" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="81" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B81" s="14" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="82" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B82" s="14" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="83" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B83" s="14" t="s">
+        <v>53</v>
       </c>
     </row>
   </sheetData>

</xml_diff>